<commit_message>
Enable non-blocking parallel processing of ticket codes
</commit_message>
<xml_diff>
--- a/Ticketcodes.xlsx
+++ b/Ticketcodes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -80,13 +80,16 @@
     <t xml:space="preserve">ph1XVUPXX3FHQN8VDU2 </t>
   </si>
   <si>
+    <t xml:space="preserve">ph1XVYUGD7DMVEUXPQN </t>
+  </si>
+  <si>
     <t xml:space="preserve">ph1XVUW9PQMTT93MWH6 </t>
   </si>
   <si>
     <t xml:space="preserve">ph1XVYHUX2EGAF6EADT </t>
   </si>
   <si>
-    <t xml:space="preserve">ph1XVYUGD7DMVEUXPQN </t>
+    <t xml:space="preserve">ph1XW2MMXQCNWMUS3U9 </t>
   </si>
   <si>
     <t xml:space="preserve">ph1XW23EFK24T8N5QWE </t>
@@ -95,28 +98,22 @@
     <t xml:space="preserve">ph1XW2GLHFFVY99CT8B </t>
   </si>
   <si>
-    <t xml:space="preserve">ph1XW2MMXQCNWMUS3U9 </t>
-  </si>
-  <si>
     <t xml:space="preserve">ph1XW33CL8QB9ZQ92MN </t>
   </si>
   <si>
     <t xml:space="preserve">ph1XW35LMUKLRV9FNKM </t>
   </si>
   <si>
+    <t xml:space="preserve">ph1XW8DAALMAUU4E47Y </t>
+  </si>
+  <si>
     <t xml:space="preserve">ph1XW3VCA7ZBCNZB9CP </t>
   </si>
   <si>
     <t xml:space="preserve">ph1XW5PPMWDAYAYDFPQ </t>
   </si>
   <si>
-    <t xml:space="preserve">ph1XW8DAALMAUU4E47Y </t>
-  </si>
-  <si>
     <t>eingelöst</t>
-  </si>
-  <si>
-    <t>sni</t>
   </si>
 </sst>
 </file>
@@ -474,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -636,11 +633,6 @@
       </c>
       <c r="F13" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="20:20">
-      <c r="T25" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>